<commit_message>
Trained decision tree models, however not yet integrated for results.
</commit_message>
<xml_diff>
--- a/results/models.xlsx
+++ b/results/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\XAI_time_series\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9E4F1A-E0FD-4F06-805F-0F80C654D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83867452-20A7-4B3F-B149-97F503B9132D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>cnn</t>
+  </si>
+  <si>
+    <t>decision_tree</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +461,38 @@
         <v>0.62829405069351196</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.99019607843137203</v>
+      </c>
+      <c r="D3">
+        <v>0.95850622406638997</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.87337662337662303</v>
+      </c>
+      <c r="J3">
+        <v>0.62552011095700399</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented Linear Regression and running results for models and datasets.
</commit_message>
<xml_diff>
--- a/results/models.xlsx
+++ b/results/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\XAI_time_series\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83867452-20A7-4B3F-B149-97F503B9132D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556A6C37-0C0A-492D-83F2-D46DFA51CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,42 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
   <si>
-    <t>Chinatown Train</t>
-  </si>
-  <si>
-    <t>Chinatown Val</t>
-  </si>
-  <si>
-    <t>Chinatown Test</t>
-  </si>
-  <si>
-    <t>ECG200 Train</t>
-  </si>
-  <si>
-    <t>ECG200 Val</t>
-  </si>
-  <si>
-    <t>ECG200 Test</t>
-  </si>
-  <si>
-    <t>ItalyPowerDemand Train</t>
-  </si>
-  <si>
-    <t>ItalyPowerDemand Val</t>
-  </si>
-  <si>
-    <t>ItalyPowerDemand Test</t>
-  </si>
-  <si>
     <t>cnn</t>
   </si>
   <si>
-    <t>decision_tree</t>
+    <t>linear-regression</t>
+  </si>
+  <si>
+    <t>decision-tree</t>
+  </si>
+  <si>
+    <t>Chinatown Train (accuracy)</t>
+  </si>
+  <si>
+    <t>Chinatown Val (accuracy)</t>
+  </si>
+  <si>
+    <t>Chinatown Test (accuracy)</t>
+  </si>
+  <si>
+    <t>ECG200 Train (accuracy)</t>
+  </si>
+  <si>
+    <t>ECG200 Val (accuracy)</t>
+  </si>
+  <si>
+    <t>ECG200 Test (accuracy)</t>
+  </si>
+  <si>
+    <t>ItalyPowerDemand Train (accuracy)</t>
+  </si>
+  <si>
+    <t>ItalyPowerDemand Val (accuracy)</t>
+  </si>
+  <si>
+    <t>ItalyPowerDemand Test (accuracy)</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,36 +405,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0.98600000143051103</v>
@@ -463,7 +466,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -491,6 +494,38 @@
       </c>
       <c r="J3">
         <v>0.62552011095700399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.86274509803921495</v>
+      </c>
+      <c r="D4">
+        <v>0.89211618257261405</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="G4">
+        <v>0.28571428571428498</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0.50324675324675305</v>
+      </c>
+      <c r="J4">
+        <v>0.50069348127600499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>